<commit_message>
cedula por linea y no general en activador
</commit_message>
<xml_diff>
--- a/src/preactivador/preactivador.xlsx
+++ b/src/preactivador/preactivador.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Olimpostudio\Temporales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\TeamComunicaciones\automatizadorteam\src\preactivador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C9DFFC-D265-4CDB-AEAC-62944DA1C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437C3D3F-784D-4A7B-9C81-34E7A88318E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="3015" windowWidth="13005" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Iccid</t>
+  </si>
+  <si>
+    <t>Nit</t>
+  </si>
+  <si>
+    <t>Cedula</t>
   </si>
   <si>
     <t>Min</t>
   </si>
   <si>
     <t>Mensaje</t>
-  </si>
-  <si>
-    <t>Nit</t>
   </si>
 </sst>
 </file>
@@ -394,18 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -413,10 +413,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>